<commit_message>
modified responses in xlsx
</commit_message>
<xml_diff>
--- a/responses.xlsx
+++ b/responses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshvasilvasstar/Documents/clinicchat/ibm_watson_uploads/c4h/salud/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joshvasilvasstar/Documents/clinicchat/sa-c4h-project/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E54827-6F03-5B4D-94A4-8C34910E1EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D329C416-DC1D-D64F-8DE2-701BD9037ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="7580" windowWidth="27640" windowHeight="16940" xr2:uid="{E7C9F955-17B0-F040-8EA4-EA009C6A7680}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2566" uniqueCount="1184">
   <si>
     <t>Why should I eat healthy food?</t>
   </si>
@@ -4024,6 +4024,9 @@
   </si>
   <si>
     <t>How can I prevent diabetes, high blood pressure, and high blood cholesterol?</t>
+  </si>
+  <si>
+    <t>Si tiene varias condiciones medicas, deberá hacer un seguimiento con todas y aun mas con su diabetes. Siga las indicaciones de su proveedor para continuar una vida saludable y agradable.</t>
   </si>
 </sst>
 </file>
@@ -4221,7 +4224,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -4239,22 +4242,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFC7CE"/>
-          <bgColor rgb="FF000000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4588,10 +4575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F216" sqref="F216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4626,7 +4614,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" hidden="1">
       <c r="A2" s="9" t="s">
         <v>386</v>
       </c>
@@ -4652,7 +4640,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" hidden="1">
       <c r="A3" s="9" t="s">
         <v>386</v>
       </c>
@@ -4678,7 +4666,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" hidden="1">
       <c r="A4" s="9" t="s">
         <v>393</v>
       </c>
@@ -4704,7 +4692,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" hidden="1">
       <c r="A5" s="9" t="s">
         <v>393</v>
       </c>
@@ -4730,7 +4718,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" hidden="1">
       <c r="A6" s="9" t="s">
         <v>393</v>
       </c>
@@ -4756,7 +4744,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" hidden="1">
       <c r="A7" s="9" t="s">
         <v>393</v>
       </c>
@@ -4782,7 +4770,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" hidden="1">
       <c r="A8" s="9" t="s">
         <v>393</v>
       </c>
@@ -4808,7 +4796,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" hidden="1">
       <c r="A9" s="9" t="s">
         <v>393</v>
       </c>
@@ -4834,7 +4822,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" hidden="1">
       <c r="A10" s="9" t="s">
         <v>393</v>
       </c>
@@ -4860,7 +4848,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" hidden="1">
       <c r="A11" s="9" t="s">
         <v>385</v>
       </c>
@@ -4886,7 +4874,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" hidden="1">
       <c r="A12" s="9" t="s">
         <v>385</v>
       </c>
@@ -4912,7 +4900,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" hidden="1">
       <c r="A13" s="9" t="s">
         <v>385</v>
       </c>
@@ -4938,7 +4926,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" hidden="1">
       <c r="A14" s="9" t="s">
         <v>385</v>
       </c>
@@ -4964,7 +4952,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" hidden="1">
       <c r="A15" s="9" t="s">
         <v>385</v>
       </c>
@@ -4990,7 +4978,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" hidden="1">
       <c r="A16" s="9" t="s">
         <v>385</v>
       </c>
@@ -5016,7 +5004,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" hidden="1">
       <c r="A17" s="9" t="s">
         <v>385</v>
       </c>
@@ -5042,7 +5030,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" hidden="1">
       <c r="A18" s="9" t="s">
         <v>385</v>
       </c>
@@ -5068,7 +5056,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" hidden="1">
       <c r="A19" s="9" t="s">
         <v>385</v>
       </c>
@@ -5094,7 +5082,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" hidden="1">
       <c r="A20" s="9" t="s">
         <v>385</v>
       </c>
@@ -5120,7 +5108,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" hidden="1">
       <c r="A21" s="9" t="s">
         <v>385</v>
       </c>
@@ -5146,7 +5134,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" hidden="1">
       <c r="A22" s="9" t="s">
         <v>385</v>
       </c>
@@ -5172,7 +5160,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" hidden="1">
       <c r="A23" s="9" t="s">
         <v>385</v>
       </c>
@@ -5198,7 +5186,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" hidden="1">
       <c r="A24" s="9" t="s">
         <v>385</v>
       </c>
@@ -5224,7 +5212,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" hidden="1">
       <c r="A25" s="9" t="s">
         <v>385</v>
       </c>
@@ -5250,7 +5238,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" hidden="1">
       <c r="A26" s="9" t="s">
         <v>385</v>
       </c>
@@ -5276,7 +5264,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" hidden="1">
       <c r="A27" s="9" t="s">
         <v>385</v>
       </c>
@@ -5302,7 +5290,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" hidden="1">
       <c r="A28" s="9" t="s">
         <v>385</v>
       </c>
@@ -5328,7 +5316,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" hidden="1">
       <c r="A29" s="9" t="s">
         <v>385</v>
       </c>
@@ -5354,7 +5342,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" hidden="1">
       <c r="A30" s="9" t="s">
         <v>386</v>
       </c>
@@ -5380,7 +5368,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" hidden="1">
       <c r="A31" s="9" t="s">
         <v>386</v>
       </c>
@@ -5406,7 +5394,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" hidden="1">
       <c r="A32" s="9" t="s">
         <v>386</v>
       </c>
@@ -5432,7 +5420,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" hidden="1">
       <c r="A33" s="9" t="s">
         <v>386</v>
       </c>
@@ -5458,7 +5446,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" hidden="1">
       <c r="A34" s="9" t="s">
         <v>386</v>
       </c>
@@ -5484,7 +5472,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" hidden="1">
       <c r="A35" s="9" t="s">
         <v>386</v>
       </c>
@@ -5510,7 +5498,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" hidden="1">
       <c r="A36" s="9" t="s">
         <v>386</v>
       </c>
@@ -5536,7 +5524,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" hidden="1">
       <c r="A37" s="9" t="s">
         <v>386</v>
       </c>
@@ -5562,7 +5550,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" hidden="1">
       <c r="A38" s="9" t="s">
         <v>386</v>
       </c>
@@ -5588,7 +5576,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" hidden="1">
       <c r="A39" s="9" t="s">
         <v>386</v>
       </c>
@@ -5614,7 +5602,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" hidden="1">
       <c r="A40" s="9" t="s">
         <v>386</v>
       </c>
@@ -5640,7 +5628,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" hidden="1">
       <c r="A41" s="9" t="s">
         <v>386</v>
       </c>
@@ -5666,7 +5654,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" hidden="1">
       <c r="A42" s="9" t="s">
         <v>386</v>
       </c>
@@ -5692,7 +5680,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" hidden="1">
       <c r="A43" s="9" t="s">
         <v>386</v>
       </c>
@@ -5718,7 +5706,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" hidden="1">
       <c r="A44" s="9" t="s">
         <v>386</v>
       </c>
@@ -5744,7 +5732,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" hidden="1">
       <c r="A45" s="9" t="s">
         <v>386</v>
       </c>
@@ -5770,7 +5758,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" hidden="1">
       <c r="A46" s="9" t="s">
         <v>386</v>
       </c>
@@ -5796,7 +5784,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" hidden="1">
       <c r="A47" s="9" t="s">
         <v>386</v>
       </c>
@@ -5822,7 +5810,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" hidden="1">
       <c r="A48" s="9" t="s">
         <v>386</v>
       </c>
@@ -5848,7 +5836,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" hidden="1">
       <c r="A49" s="9" t="s">
         <v>386</v>
       </c>
@@ -5874,7 +5862,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" hidden="1">
       <c r="A50" s="9" t="s">
         <v>386</v>
       </c>
@@ -5900,7 +5888,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" hidden="1">
       <c r="A51" s="9" t="s">
         <v>386</v>
       </c>
@@ -5926,7 +5914,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" hidden="1">
       <c r="A52" s="9" t="s">
         <v>386</v>
       </c>
@@ -5952,7 +5940,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" hidden="1">
       <c r="A53" s="9" t="s">
         <v>386</v>
       </c>
@@ -5978,7 +5966,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" hidden="1">
       <c r="A54" s="9" t="s">
         <v>386</v>
       </c>
@@ -6004,7 +5992,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" hidden="1">
       <c r="A55" s="9" t="s">
         <v>386</v>
       </c>
@@ -6030,7 +6018,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" hidden="1">
       <c r="A56" s="9" t="s">
         <v>386</v>
       </c>
@@ -6056,7 +6044,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" hidden="1">
       <c r="A57" s="9" t="s">
         <v>386</v>
       </c>
@@ -6082,7 +6070,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" hidden="1">
       <c r="A58" s="9" t="s">
         <v>386</v>
       </c>
@@ -6108,7 +6096,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" hidden="1">
       <c r="A59" s="9" t="s">
         <v>387</v>
       </c>
@@ -6134,7 +6122,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" hidden="1">
       <c r="A60" s="9" t="s">
         <v>387</v>
       </c>
@@ -6160,7 +6148,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" hidden="1">
       <c r="A61" s="9" t="s">
         <v>387</v>
       </c>
@@ -6186,7 +6174,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" hidden="1">
       <c r="A62" s="9" t="s">
         <v>387</v>
       </c>
@@ -6212,7 +6200,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" hidden="1">
       <c r="A63" s="9" t="s">
         <v>387</v>
       </c>
@@ -6238,7 +6226,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" hidden="1">
       <c r="A64" s="9" t="s">
         <v>387</v>
       </c>
@@ -6264,7 +6252,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" hidden="1">
       <c r="A65" s="9" t="s">
         <v>387</v>
       </c>
@@ -6290,7 +6278,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" hidden="1">
       <c r="A66" s="9" t="s">
         <v>387</v>
       </c>
@@ -6316,7 +6304,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" hidden="1">
       <c r="A67" s="9" t="s">
         <v>388</v>
       </c>
@@ -6342,7 +6330,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" hidden="1">
       <c r="A68" s="9" t="s">
         <v>388</v>
       </c>
@@ -6368,7 +6356,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" hidden="1">
       <c r="A69" s="9" t="s">
         <v>388</v>
       </c>
@@ -6394,7 +6382,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" hidden="1">
       <c r="A70" s="9" t="s">
         <v>388</v>
       </c>
@@ -6420,7 +6408,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" hidden="1">
       <c r="A71" s="9" t="s">
         <v>388</v>
       </c>
@@ -6446,7 +6434,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" hidden="1">
       <c r="A72" s="9" t="s">
         <v>388</v>
       </c>
@@ -6472,7 +6460,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" hidden="1">
       <c r="A73" s="9" t="s">
         <v>388</v>
       </c>
@@ -6498,7 +6486,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" hidden="1">
       <c r="A74" s="9" t="s">
         <v>388</v>
       </c>
@@ -6524,7 +6512,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" hidden="1">
       <c r="A75" s="9" t="s">
         <v>388</v>
       </c>
@@ -6550,7 +6538,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" hidden="1">
       <c r="A76" s="9" t="s">
         <v>388</v>
       </c>
@@ -6576,7 +6564,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" hidden="1">
       <c r="A77" s="9" t="s">
         <v>388</v>
       </c>
@@ -6602,7 +6590,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" hidden="1">
       <c r="A78" s="9" t="s">
         <v>388</v>
       </c>
@@ -6628,7 +6616,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" hidden="1">
       <c r="A79" s="9" t="s">
         <v>389</v>
       </c>
@@ -6654,7 +6642,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" hidden="1">
       <c r="A80" s="9" t="s">
         <v>389</v>
       </c>
@@ -6680,7 +6668,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" hidden="1">
       <c r="A81" s="9" t="s">
         <v>389</v>
       </c>
@@ -6706,7 +6694,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" hidden="1">
       <c r="A82" s="9" t="s">
         <v>389</v>
       </c>
@@ -6732,7 +6720,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" hidden="1">
       <c r="A83" s="9" t="s">
         <v>389</v>
       </c>
@@ -6758,7 +6746,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" hidden="1">
       <c r="A84" s="9" t="s">
         <v>389</v>
       </c>
@@ -6784,7 +6772,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" hidden="1">
       <c r="A85" s="9" t="s">
         <v>389</v>
       </c>
@@ -6810,7 +6798,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" hidden="1">
       <c r="A86" s="9" t="s">
         <v>389</v>
       </c>
@@ -6836,7 +6824,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" hidden="1">
       <c r="A87" s="9" t="s">
         <v>390</v>
       </c>
@@ -6862,7 +6850,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" hidden="1">
       <c r="A88" s="9" t="s">
         <v>390</v>
       </c>
@@ -6888,7 +6876,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" hidden="1">
       <c r="A89" s="9" t="s">
         <v>390</v>
       </c>
@@ -6914,7 +6902,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" hidden="1">
       <c r="A90" s="9" t="s">
         <v>390</v>
       </c>
@@ -6940,7 +6928,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" hidden="1">
       <c r="A91" s="9" t="s">
         <v>390</v>
       </c>
@@ -6966,7 +6954,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" hidden="1">
       <c r="A92" s="9" t="s">
         <v>390</v>
       </c>
@@ -6992,7 +6980,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" hidden="1">
       <c r="A93" s="9" t="s">
         <v>390</v>
       </c>
@@ -7018,7 +7006,7 @@
         <v>839</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" hidden="1">
       <c r="A94" s="9" t="s">
         <v>390</v>
       </c>
@@ -7044,7 +7032,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" hidden="1">
       <c r="A95" s="9" t="s">
         <v>390</v>
       </c>
@@ -7070,7 +7058,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" hidden="1">
       <c r="A96" s="9" t="s">
         <v>390</v>
       </c>
@@ -7096,7 +7084,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" hidden="1">
       <c r="A97" s="9" t="s">
         <v>390</v>
       </c>
@@ -7122,7 +7110,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" hidden="1">
       <c r="A98" s="9" t="s">
         <v>390</v>
       </c>
@@ -7148,7 +7136,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" hidden="1">
       <c r="A99" s="9" t="s">
         <v>390</v>
       </c>
@@ -7174,7 +7162,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" hidden="1">
       <c r="A100" s="9" t="s">
         <v>390</v>
       </c>
@@ -7200,7 +7188,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" hidden="1">
       <c r="A101" s="9" t="s">
         <v>390</v>
       </c>
@@ -7226,7 +7214,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" hidden="1">
       <c r="A102" s="9" t="s">
         <v>391</v>
       </c>
@@ -7252,7 +7240,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" hidden="1">
       <c r="A103" s="9" t="s">
         <v>391</v>
       </c>
@@ -7278,7 +7266,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" hidden="1">
       <c r="A104" s="9" t="s">
         <v>391</v>
       </c>
@@ -7304,7 +7292,7 @@
         <v>852</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" hidden="1">
       <c r="A105" s="9" t="s">
         <v>391</v>
       </c>
@@ -7330,7 +7318,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" hidden="1">
       <c r="A106" s="9" t="s">
         <v>391</v>
       </c>
@@ -7356,7 +7344,7 @@
         <v>854</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" hidden="1">
       <c r="A107" s="9" t="s">
         <v>391</v>
       </c>
@@ -7382,7 +7370,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" hidden="1">
       <c r="A108" s="9" t="s">
         <v>391</v>
       </c>
@@ -7408,7 +7396,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" hidden="1">
       <c r="A109" s="9" t="s">
         <v>391</v>
       </c>
@@ -7434,7 +7422,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" hidden="1">
       <c r="A110" s="9" t="s">
         <v>391</v>
       </c>
@@ -7460,7 +7448,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" hidden="1">
       <c r="A111" s="9" t="s">
         <v>391</v>
       </c>
@@ -7486,7 +7474,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" hidden="1">
       <c r="A112" s="9" t="s">
         <v>391</v>
       </c>
@@ -7512,7 +7500,7 @@
         <v>862</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" hidden="1">
       <c r="A113" s="9" t="s">
         <v>392</v>
       </c>
@@ -7538,7 +7526,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" hidden="1">
       <c r="A114" s="9" t="s">
         <v>392</v>
       </c>
@@ -7564,7 +7552,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" hidden="1">
       <c r="A115" s="9" t="s">
         <v>392</v>
       </c>
@@ -7590,7 +7578,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" hidden="1">
       <c r="A116" s="9" t="s">
         <v>392</v>
       </c>
@@ -7616,7 +7604,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" hidden="1">
       <c r="A117" s="9" t="s">
         <v>392</v>
       </c>
@@ -7642,7 +7630,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" hidden="1">
       <c r="A118" s="9" t="s">
         <v>392</v>
       </c>
@@ -7668,7 +7656,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" hidden="1">
       <c r="A119" s="9" t="s">
         <v>392</v>
       </c>
@@ -7694,7 +7682,7 @@
         <v>870</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" hidden="1">
       <c r="A120" s="9" t="s">
         <v>392</v>
       </c>
@@ -7720,7 +7708,7 @@
         <v>871</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" hidden="1">
       <c r="A121" s="9" t="s">
         <v>392</v>
       </c>
@@ -7746,7 +7734,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" hidden="1">
       <c r="A122" s="9" t="s">
         <v>393</v>
       </c>
@@ -7772,7 +7760,7 @@
         <v>873</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" hidden="1">
       <c r="A123" s="9" t="s">
         <v>393</v>
       </c>
@@ -7798,7 +7786,7 @@
         <v>874</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" hidden="1">
       <c r="A124" s="9" t="s">
         <v>393</v>
       </c>
@@ -7824,7 +7812,7 @@
         <v>875</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" hidden="1">
       <c r="A125" s="9" t="s">
         <v>393</v>
       </c>
@@ -7850,7 +7838,7 @@
         <v>877</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" hidden="1">
       <c r="A126" s="9" t="s">
         <v>393</v>
       </c>
@@ -7876,7 +7864,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" hidden="1">
       <c r="A127" s="9" t="s">
         <v>393</v>
       </c>
@@ -7902,7 +7890,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" hidden="1">
       <c r="A128" s="9" t="s">
         <v>393</v>
       </c>
@@ -7928,7 +7916,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" hidden="1">
       <c r="A129" s="9" t="s">
         <v>393</v>
       </c>
@@ -7954,7 +7942,7 @@
         <v>881</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" hidden="1">
       <c r="A130" s="9" t="s">
         <v>393</v>
       </c>
@@ -7980,7 +7968,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" hidden="1">
       <c r="A131" s="9" t="s">
         <v>393</v>
       </c>
@@ -8006,7 +7994,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" hidden="1">
       <c r="A132" s="9" t="s">
         <v>393</v>
       </c>
@@ -8032,7 +8020,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" hidden="1">
       <c r="A133" s="9" t="s">
         <v>393</v>
       </c>
@@ -8058,7 +8046,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" hidden="1">
       <c r="A134" s="9" t="s">
         <v>393</v>
       </c>
@@ -8084,7 +8072,7 @@
         <v>892</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" hidden="1">
       <c r="A135" s="9" t="s">
         <v>393</v>
       </c>
@@ -8110,7 +8098,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" hidden="1">
       <c r="A136" s="9" t="s">
         <v>393</v>
       </c>
@@ -8136,7 +8124,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" hidden="1">
       <c r="A137" s="9" t="s">
         <v>393</v>
       </c>
@@ -8162,7 +8150,7 @@
         <v>898</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" hidden="1">
       <c r="A138" s="9" t="s">
         <v>393</v>
       </c>
@@ -8188,7 +8176,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" hidden="1">
       <c r="A139" s="9" t="s">
         <v>393</v>
       </c>
@@ -8214,7 +8202,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" hidden="1">
       <c r="A140" s="9" t="s">
         <v>393</v>
       </c>
@@ -8240,7 +8228,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" hidden="1">
       <c r="A141" s="9" t="s">
         <v>393</v>
       </c>
@@ -8266,7 +8254,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" hidden="1">
       <c r="A142" s="9" t="s">
         <v>393</v>
       </c>
@@ -8292,7 +8280,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" hidden="1">
       <c r="A143" s="9" t="s">
         <v>393</v>
       </c>
@@ -8318,7 +8306,7 @@
         <v>912</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" hidden="1">
       <c r="A144" s="9" t="s">
         <v>393</v>
       </c>
@@ -8344,7 +8332,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" hidden="1">
       <c r="A145" s="9" t="s">
         <v>393</v>
       </c>
@@ -8370,7 +8358,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" hidden="1">
       <c r="A146" s="9" t="s">
         <v>393</v>
       </c>
@@ -8396,7 +8384,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" hidden="1">
       <c r="A147" s="9" t="s">
         <v>393</v>
       </c>
@@ -8422,7 +8410,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" hidden="1">
       <c r="A148" s="9" t="s">
         <v>393</v>
       </c>
@@ -8448,7 +8436,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" hidden="1">
       <c r="A149" s="9" t="s">
         <v>393</v>
       </c>
@@ -8474,7 +8462,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" hidden="1">
       <c r="A150" s="9" t="s">
         <v>393</v>
       </c>
@@ -8500,7 +8488,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" hidden="1">
       <c r="A151" s="9" t="s">
         <v>393</v>
       </c>
@@ -8526,7 +8514,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" hidden="1">
       <c r="A152" s="9" t="s">
         <v>393</v>
       </c>
@@ -8552,7 +8540,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" hidden="1">
       <c r="A153" s="9" t="s">
         <v>393</v>
       </c>
@@ -8578,7 +8566,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" hidden="1">
       <c r="A154" s="9" t="s">
         <v>393</v>
       </c>
@@ -8604,7 +8592,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" hidden="1">
       <c r="A155" s="9" t="s">
         <v>393</v>
       </c>
@@ -8630,7 +8618,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" hidden="1">
       <c r="A156" s="9" t="s">
         <v>393</v>
       </c>
@@ -8656,7 +8644,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" hidden="1">
       <c r="A157" s="9" t="s">
         <v>393</v>
       </c>
@@ -8682,7 +8670,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" hidden="1">
       <c r="A158" s="9" t="s">
         <v>393</v>
       </c>
@@ -8708,7 +8696,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" hidden="1">
       <c r="A159" s="9" t="s">
         <v>393</v>
       </c>
@@ -8734,7 +8722,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" hidden="1">
       <c r="A160" s="9" t="s">
         <v>393</v>
       </c>
@@ -8760,7 +8748,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" hidden="1">
       <c r="A161" s="9" t="s">
         <v>393</v>
       </c>
@@ -8786,7 +8774,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" hidden="1">
       <c r="A162" s="9" t="s">
         <v>393</v>
       </c>
@@ -8812,7 +8800,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" hidden="1">
       <c r="A163" s="9" t="s">
         <v>393</v>
       </c>
@@ -8838,7 +8826,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" hidden="1">
       <c r="A164" s="9" t="s">
         <v>393</v>
       </c>
@@ -8864,7 +8852,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" hidden="1">
       <c r="A165" s="9" t="s">
         <v>393</v>
       </c>
@@ -8890,7 +8878,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" hidden="1">
       <c r="A166" s="9" t="s">
         <v>393</v>
       </c>
@@ -8916,7 +8904,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" hidden="1">
       <c r="A167" s="9" t="s">
         <v>393</v>
       </c>
@@ -8942,7 +8930,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" hidden="1">
       <c r="A168" s="9" t="s">
         <v>393</v>
       </c>
@@ -8968,7 +8956,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" hidden="1">
       <c r="A169" s="9" t="s">
         <v>393</v>
       </c>
@@ -8994,7 +8982,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" hidden="1">
       <c r="A170" s="9" t="s">
         <v>393</v>
       </c>
@@ -9020,7 +9008,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" hidden="1">
       <c r="A171" s="9" t="s">
         <v>393</v>
       </c>
@@ -9046,7 +9034,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" hidden="1">
       <c r="A172" s="9" t="s">
         <v>393</v>
       </c>
@@ -9072,7 +9060,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" hidden="1">
       <c r="A173" s="9" t="s">
         <v>393</v>
       </c>
@@ -9098,7 +9086,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" hidden="1">
       <c r="A174" s="9" t="s">
         <v>393</v>
       </c>
@@ -9124,7 +9112,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" hidden="1">
       <c r="A175" s="9" t="s">
         <v>393</v>
       </c>
@@ -9150,7 +9138,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" hidden="1">
       <c r="A176" s="9" t="s">
         <v>393</v>
       </c>
@@ -9176,7 +9164,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" hidden="1">
       <c r="A177" s="9" t="s">
         <v>393</v>
       </c>
@@ -9202,7 +9190,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" hidden="1">
       <c r="A178" s="9" t="s">
         <v>393</v>
       </c>
@@ -9228,7 +9216,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" hidden="1">
       <c r="A179" s="9" t="s">
         <v>393</v>
       </c>
@@ -9254,7 +9242,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" hidden="1">
       <c r="A180" s="9" t="s">
         <v>393</v>
       </c>
@@ -9280,7 +9268,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" hidden="1">
       <c r="A181" s="9" t="s">
         <v>393</v>
       </c>
@@ -9306,7 +9294,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" hidden="1">
       <c r="A182" s="9" t="s">
         <v>393</v>
       </c>
@@ -9332,7 +9320,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" hidden="1">
       <c r="A183" s="9" t="s">
         <v>393</v>
       </c>
@@ -9358,7 +9346,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" hidden="1">
       <c r="A184" s="9" t="s">
         <v>393</v>
       </c>
@@ -9384,7 +9372,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" hidden="1">
       <c r="A185" s="9" t="s">
         <v>393</v>
       </c>
@@ -9410,7 +9398,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" hidden="1">
       <c r="A186" s="9" t="s">
         <v>393</v>
       </c>
@@ -9436,7 +9424,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" hidden="1">
       <c r="A187" s="9" t="s">
         <v>393</v>
       </c>
@@ -9462,7 +9450,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" hidden="1">
       <c r="A188" s="9" t="s">
         <v>393</v>
       </c>
@@ -9488,7 +9476,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" hidden="1">
       <c r="A189" s="9" t="s">
         <v>393</v>
       </c>
@@ -9514,7 +9502,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" hidden="1">
       <c r="A190" s="9" t="s">
         <v>393</v>
       </c>
@@ -9540,7 +9528,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" hidden="1">
       <c r="A191" s="9" t="s">
         <v>393</v>
       </c>
@@ -9566,7 +9554,7 @@
         <v>1031</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" hidden="1">
       <c r="A192" s="9" t="s">
         <v>393</v>
       </c>
@@ -9592,7 +9580,7 @@
         <v>1034</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" hidden="1">
       <c r="A193" s="9" t="s">
         <v>393</v>
       </c>
@@ -9618,7 +9606,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" hidden="1">
       <c r="A194" s="9" t="s">
         <v>393</v>
       </c>
@@ -9644,7 +9632,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" hidden="1">
       <c r="A195" s="9" t="s">
         <v>393</v>
       </c>
@@ -9670,7 +9658,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" hidden="1">
       <c r="A196" s="9" t="s">
         <v>393</v>
       </c>
@@ -9696,7 +9684,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" hidden="1">
       <c r="A197" s="9" t="s">
         <v>393</v>
       </c>
@@ -9722,7 +9710,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" hidden="1">
       <c r="A198" s="9" t="s">
         <v>393</v>
       </c>
@@ -9748,7 +9736,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" hidden="1">
       <c r="A199" s="9" t="s">
         <v>393</v>
       </c>
@@ -9774,7 +9762,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" hidden="1">
       <c r="A200" s="9" t="s">
         <v>393</v>
       </c>
@@ -9800,7 +9788,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" hidden="1">
       <c r="A201" s="9" t="s">
         <v>393</v>
       </c>
@@ -9826,7 +9814,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" hidden="1">
       <c r="A202" s="9" t="s">
         <v>393</v>
       </c>
@@ -9852,7 +9840,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" hidden="1">
       <c r="A203" s="9" t="s">
         <v>393</v>
       </c>
@@ -9878,7 +9866,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" hidden="1">
       <c r="A204" s="9" t="s">
         <v>393</v>
       </c>
@@ -9904,7 +9892,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" hidden="1">
       <c r="A205" s="9" t="s">
         <v>393</v>
       </c>
@@ -9930,7 +9918,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" hidden="1">
       <c r="A206" s="9" t="s">
         <v>393</v>
       </c>
@@ -9956,7 +9944,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" hidden="1">
       <c r="A207" s="9" t="s">
         <v>393</v>
       </c>
@@ -9982,7 +9970,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" hidden="1">
       <c r="A208" s="9" t="s">
         <v>393</v>
       </c>
@@ -10008,7 +9996,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" hidden="1">
       <c r="A209" s="9" t="s">
         <v>393</v>
       </c>
@@ -10034,7 +10022,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" hidden="1">
       <c r="A210" s="9" t="s">
         <v>393</v>
       </c>
@@ -10060,7 +10048,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" hidden="1">
       <c r="A211" s="9" t="s">
         <v>393</v>
       </c>
@@ -10086,7 +10074,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" hidden="1">
       <c r="A212" s="9" t="s">
         <v>393</v>
       </c>
@@ -10112,7 +10100,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" hidden="1">
       <c r="A213" s="9" t="s">
         <v>393</v>
       </c>
@@ -10138,7 +10126,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" hidden="1">
       <c r="A214" s="9" t="s">
         <v>393</v>
       </c>
@@ -10164,7 +10152,7 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" hidden="1">
       <c r="A215" s="9" t="s">
         <v>393</v>
       </c>
@@ -10206,8 +10194,8 @@
       <c r="E216" t="s">
         <v>1116</v>
       </c>
-      <c r="F216">
-        <v>0</v>
+      <c r="F216" s="16" t="s">
+        <v>1183</v>
       </c>
       <c r="G216" s="1" t="s">
         <v>404</v>
@@ -10216,7 +10204,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" hidden="1">
       <c r="A217" s="9" t="s">
         <v>393</v>
       </c>
@@ -10242,7 +10230,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" hidden="1">
       <c r="A218" s="9" t="s">
         <v>393</v>
       </c>
@@ -10268,7 +10256,7 @@
         <v>1125</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" hidden="1">
       <c r="A219" s="9" t="s">
         <v>393</v>
       </c>
@@ -10295,11 +10283,18 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H219" xr:uid="{0FC232BA-84F4-BE49-B367-4C71587DA4B6}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C16" r:id="rId1" display="https://www.mayoclinic.org/healthy-lifestyle/recipes/chicken-fajitas/rcp-20049943." xr:uid="{BF040B87-8534-9445-90AC-FE2659D40410}"/>

</xml_diff>